<commit_message>
reduce granularity to 1s/5s, change enjoiyment columns
</commit_message>
<xml_diff>
--- a/MFQS walking questionnaire 2.xlsx
+++ b/MFQS walking questionnaire 2.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="23">
   <si>
     <t>Tijdstempel</t>
   </si>
@@ -29,6 +29,42 @@
     <t>hate-enjoy</t>
   </si>
   <si>
+    <t>notpleasant_pleasant</t>
+  </si>
+  <si>
+    <t>notpleasurable_pleasurable</t>
+  </si>
+  <si>
+    <t>bad-good_feeling</t>
+  </si>
+  <si>
+    <t>Weather</t>
+  </si>
+  <si>
+    <t>Temperature (Celsius)</t>
+  </si>
+  <si>
+    <t>UV index</t>
+  </si>
+  <si>
+    <t>Wind (m/s)</t>
+  </si>
+  <si>
+    <t>Humidity (%)</t>
+  </si>
+  <si>
+    <t>Sunny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sunny </t>
+  </si>
+  <si>
+    <t>Cloudy</t>
+  </si>
+  <si>
+    <t>4.44</t>
+  </si>
+  <si>
     <t>bored-interested</t>
   </si>
   <si>
@@ -45,36 +81,6 @@
   </si>
   <si>
     <t>sense_accomplishment</t>
-  </si>
-  <si>
-    <t>Weather</t>
-  </si>
-  <si>
-    <t>Temperature (Celsius)</t>
-  </si>
-  <si>
-    <t>UV index</t>
-  </si>
-  <si>
-    <t>Wind (m/s)</t>
-  </si>
-  <si>
-    <t>Humidity (%)</t>
-  </si>
-  <si>
-    <t>Sunny</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sunny </t>
-  </si>
-  <si>
-    <t>Cloudy</t>
-  </si>
-  <si>
-    <t>low</t>
-  </si>
-  <si>
-    <t>moderate</t>
   </si>
 </sst>
 </file>
@@ -84,7 +90,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -95,6 +101,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -130,6 +144,15 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="19" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="19" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -354,7 +377,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="18" width="18.88"/>
+    <col customWidth="1" min="1" max="15" width="18.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -373,22 +396,22 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
@@ -396,15 +419,6 @@
       </c>
       <c r="M1" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2">
@@ -423,37 +437,28 @@
       <c r="E2" s="4">
         <v>4.0</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="7">
         <v>4.0</v>
       </c>
       <c r="G2" s="4">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="H2" s="4">
         <v>4.0</v>
       </c>
-      <c r="I2" s="4">
-        <v>4.0</v>
+      <c r="I2" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J2" s="4">
-        <v>4.0</v>
+        <v>21.0</v>
       </c>
       <c r="K2" s="4">
         <v>3.0</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>16</v>
+      <c r="L2" s="4">
+        <v>5.0</v>
       </c>
       <c r="M2" s="4">
-        <v>21.0</v>
-      </c>
-      <c r="N2" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="O2" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="P2" s="4">
         <v>54.0</v>
       </c>
     </row>
@@ -473,8 +478,8 @@
       <c r="E3" s="4">
         <v>4.0</v>
       </c>
-      <c r="F3" s="4">
-        <v>4.0</v>
+      <c r="F3" s="7">
+        <v>3.0</v>
       </c>
       <c r="G3" s="4">
         <v>4.0</v>
@@ -482,28 +487,19 @@
       <c r="H3" s="4">
         <v>3.0</v>
       </c>
-      <c r="I3" s="4">
-        <v>4.0</v>
+      <c r="I3" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="J3" s="4">
-        <v>3.0</v>
+        <v>22.0</v>
       </c>
       <c r="K3" s="4">
         <v>3.0</v>
       </c>
-      <c r="L3" s="4" t="s">
-        <v>17</v>
+      <c r="L3" s="4">
+        <v>5.0</v>
       </c>
       <c r="M3" s="4">
-        <v>22.0</v>
-      </c>
-      <c r="N3" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="O3" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="P3" s="4">
         <v>52.0</v>
       </c>
     </row>
@@ -523,37 +519,28 @@
       <c r="E4" s="4">
         <v>3.0</v>
       </c>
-      <c r="F4" s="4">
-        <v>4.0</v>
+      <c r="F4" s="7">
+        <v>3.0</v>
       </c>
       <c r="G4" s="4">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="H4" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="I4" s="4">
-        <v>3.0</v>
+        <v>4.0</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J4" s="4">
-        <v>4.0</v>
+        <v>21.0</v>
       </c>
       <c r="K4" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>16</v>
+        <v>3.0</v>
+      </c>
+      <c r="L4" s="4">
+        <v>5.0</v>
       </c>
       <c r="M4" s="4">
-        <v>21.0</v>
-      </c>
-      <c r="N4" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="O4" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="P4" s="4">
         <v>52.0</v>
       </c>
     </row>
@@ -573,37 +560,28 @@
       <c r="E5" s="4">
         <v>2.0</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="7">
         <v>2.0</v>
       </c>
       <c r="G5" s="4">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H5" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="I5" s="4">
-        <v>3.0</v>
+        <v>3.0</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="J5" s="4">
-        <v>3.0</v>
+        <v>15.0</v>
       </c>
       <c r="K5" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>18</v>
+        <v>0.0</v>
+      </c>
+      <c r="L5" s="4">
+        <v>5.0</v>
       </c>
       <c r="M5" s="4">
-        <v>15.0</v>
-      </c>
-      <c r="N5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="O5" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="P5" s="4">
         <v>74.0</v>
       </c>
     </row>
@@ -623,8 +601,8 @@
       <c r="E6" s="4">
         <v>4.0</v>
       </c>
-      <c r="F6" s="4">
-        <v>3.0</v>
+      <c r="F6" s="7">
+        <v>4.0</v>
       </c>
       <c r="G6" s="4">
         <v>3.0</v>
@@ -632,28 +610,19 @@
       <c r="H6" s="4">
         <v>4.0</v>
       </c>
-      <c r="I6" s="4">
-        <v>3.0</v>
+      <c r="I6" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J6" s="4">
-        <v>4.0</v>
+        <v>16.0</v>
       </c>
       <c r="K6" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>16</v>
+        <v>4.0</v>
+      </c>
+      <c r="L6" s="4">
+        <v>5.0</v>
       </c>
       <c r="M6" s="4">
-        <v>16.0</v>
-      </c>
-      <c r="N6" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="O6" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="P6" s="4">
         <v>69.0</v>
       </c>
     </row>
@@ -673,37 +642,28 @@
       <c r="E7" s="4">
         <v>3.0</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="7">
         <v>2.0</v>
       </c>
       <c r="G7" s="4">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H7" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="I7" s="4">
-        <v>3.0</v>
+        <v>3.0</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J7" s="4">
-        <v>3.0</v>
+        <v>18.0</v>
       </c>
       <c r="K7" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>16</v>
+        <v>5.0</v>
+      </c>
+      <c r="L7" s="4">
+        <v>5.0</v>
       </c>
       <c r="M7" s="4">
-        <v>18.0</v>
-      </c>
-      <c r="N7" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="O7" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="P7" s="4">
         <v>64.0</v>
       </c>
     </row>
@@ -723,37 +683,28 @@
       <c r="E8" s="4">
         <v>4.0</v>
       </c>
-      <c r="F8" s="4">
-        <v>3.0</v>
+      <c r="F8" s="7">
+        <v>4.0</v>
       </c>
       <c r="G8" s="4">
         <v>3.0</v>
       </c>
       <c r="H8" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="I8" s="4">
-        <v>3.0</v>
+        <v>3.0</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J8" s="4">
-        <v>3.0</v>
+        <v>19.0</v>
       </c>
       <c r="K8" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>16</v>
+        <v>6.0</v>
+      </c>
+      <c r="L8" s="4">
+        <v>5.0</v>
       </c>
       <c r="M8" s="4">
-        <v>19.0</v>
-      </c>
-      <c r="N8" s="4">
-        <v>6.0</v>
-      </c>
-      <c r="O8" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="P8" s="4">
         <v>59.0</v>
       </c>
     </row>
@@ -773,37 +724,28 @@
       <c r="E9" s="4">
         <v>3.0</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="7">
         <v>3.0</v>
       </c>
       <c r="G9" s="4">
         <v>4.0</v>
       </c>
       <c r="H9" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="I9" s="4">
-        <v>4.0</v>
+        <v>4.0</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J9" s="4">
-        <v>4.0</v>
+        <v>22.0</v>
       </c>
       <c r="K9" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>16</v>
+        <v>2.0</v>
+      </c>
+      <c r="L9" s="4">
+        <v>7.0</v>
       </c>
       <c r="M9" s="4">
-        <v>22.0</v>
-      </c>
-      <c r="N9" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="O9" s="4">
-        <v>7.0</v>
-      </c>
-      <c r="P9" s="4">
         <v>54.0</v>
       </c>
     </row>
@@ -823,7 +765,7 @@
       <c r="E10" s="4">
         <v>4.0</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="7">
         <v>4.0</v>
       </c>
       <c r="G10" s="4">
@@ -832,28 +774,19 @@
       <c r="H10" s="4">
         <v>4.0</v>
       </c>
-      <c r="I10" s="4">
-        <v>4.0</v>
+      <c r="I10" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J10" s="4">
-        <v>4.0</v>
+        <v>22.0</v>
       </c>
       <c r="K10" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>16</v>
+        <v>1.0</v>
+      </c>
+      <c r="L10" s="4">
+        <v>7.0</v>
       </c>
       <c r="M10" s="4">
-        <v>22.0</v>
-      </c>
-      <c r="N10" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="O10" s="4">
-        <v>7.0</v>
-      </c>
-      <c r="P10" s="4">
         <v>54.0</v>
       </c>
     </row>
@@ -873,37 +806,28 @@
       <c r="E11" s="4">
         <v>4.0</v>
       </c>
-      <c r="F11" s="4">
-        <v>4.0</v>
+      <c r="F11" s="7">
+        <v>3.0</v>
       </c>
       <c r="G11" s="4">
         <v>4.0</v>
       </c>
       <c r="H11" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="I11" s="4">
-        <v>4.0</v>
+        <v>4.0</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J11" s="4">
-        <v>4.0</v>
+        <v>22.0</v>
       </c>
       <c r="K11" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>16</v>
+        <v>1.0</v>
+      </c>
+      <c r="L11" s="4">
+        <v>6.0</v>
       </c>
       <c r="M11" s="4">
-        <v>22.0</v>
-      </c>
-      <c r="N11" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="O11" s="4">
-        <v>6.0</v>
-      </c>
-      <c r="P11" s="4">
         <v>54.0</v>
       </c>
     </row>
@@ -923,37 +847,28 @@
       <c r="E12" s="4">
         <v>3.0</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="7">
         <v>3.0</v>
       </c>
       <c r="G12" s="4">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="H12" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="I12" s="4">
-        <v>4.0</v>
+        <v>4.0</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J12" s="4">
-        <v>4.0</v>
+        <v>22.0</v>
       </c>
       <c r="K12" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>16</v>
+        <v>1.0</v>
+      </c>
+      <c r="L12" s="4">
+        <v>6.0</v>
       </c>
       <c r="M12" s="4">
-        <v>22.0</v>
-      </c>
-      <c r="N12" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="O12" s="4">
-        <v>6.0</v>
-      </c>
-      <c r="P12" s="4">
         <v>54.0</v>
       </c>
     </row>
@@ -973,37 +888,28 @@
       <c r="E13" s="4">
         <v>4.0</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="7">
         <v>3.0</v>
       </c>
       <c r="G13" s="4">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="H13" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="I13" s="4">
-        <v>4.0</v>
+        <v>4.0</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J13" s="4">
-        <v>4.0</v>
+        <v>22.0</v>
       </c>
       <c r="K13" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>16</v>
+        <v>1.0</v>
+      </c>
+      <c r="L13" s="4">
+        <v>6.0</v>
       </c>
       <c r="M13" s="4">
-        <v>22.0</v>
-      </c>
-      <c r="N13" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="O13" s="4">
-        <v>6.0</v>
-      </c>
-      <c r="P13" s="4">
         <v>54.0</v>
       </c>
     </row>
@@ -1023,37 +929,28 @@
       <c r="E14" s="4">
         <v>4.0</v>
       </c>
-      <c r="F14" s="4">
-        <v>3.0</v>
+      <c r="F14" s="7">
+        <v>2.0</v>
       </c>
       <c r="G14" s="4">
         <v>3.0</v>
       </c>
       <c r="H14" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="I14" s="4">
-        <v>3.0</v>
+        <v>3.0</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J14" s="4">
-        <v>3.0</v>
+        <v>22.0</v>
       </c>
       <c r="K14" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>16</v>
+        <v>1.0</v>
+      </c>
+      <c r="L14" s="4">
+        <v>6.0</v>
       </c>
       <c r="M14" s="4">
-        <v>22.0</v>
-      </c>
-      <c r="N14" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="O14" s="4">
-        <v>6.0</v>
-      </c>
-      <c r="P14" s="4">
         <v>54.0</v>
       </c>
     </row>
@@ -1073,37 +970,28 @@
       <c r="E15" s="4">
         <v>3.0</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="7">
         <v>2.0</v>
       </c>
       <c r="G15" s="4">
         <v>3.0</v>
       </c>
       <c r="H15" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="I15" s="4">
-        <v>3.0</v>
+        <v>3.0</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J15" s="4">
-        <v>3.0</v>
+        <v>21.0</v>
       </c>
       <c r="K15" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>16</v>
+        <v>1.0</v>
+      </c>
+      <c r="L15" s="4">
+        <v>6.0</v>
       </c>
       <c r="M15" s="4">
-        <v>21.0</v>
-      </c>
-      <c r="N15" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="O15" s="4">
-        <v>6.0</v>
-      </c>
-      <c r="P15" s="4">
         <v>55.0</v>
       </c>
     </row>
@@ -1123,37 +1011,28 @@
       <c r="E16" s="4">
         <v>3.0</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="7">
         <v>2.0</v>
       </c>
       <c r="G16" s="4">
         <v>3.0</v>
       </c>
       <c r="H16" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="I16" s="4">
-        <v>3.0</v>
+        <v>4.0</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J16" s="4">
-        <v>4.0</v>
+        <v>21.0</v>
       </c>
       <c r="K16" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="L16" s="4" t="s">
-        <v>16</v>
+        <v>0.0</v>
+      </c>
+      <c r="L16" s="4">
+        <v>6.0</v>
       </c>
       <c r="M16" s="4">
-        <v>21.0</v>
-      </c>
-      <c r="N16" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="O16" s="4">
-        <v>6.0</v>
-      </c>
-      <c r="P16" s="4">
         <v>55.0</v>
       </c>
     </row>
@@ -1173,37 +1052,28 @@
       <c r="E17" s="4">
         <v>4.0</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="7">
         <v>3.0</v>
       </c>
       <c r="G17" s="4">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="H17" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="I17" s="4">
-        <v>4.0</v>
+        <v>4.0</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J17" s="4">
-        <v>4.0</v>
+        <v>20.0</v>
       </c>
       <c r="K17" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>16</v>
+        <v>0.0</v>
+      </c>
+      <c r="L17" s="4">
+        <v>6.0</v>
       </c>
       <c r="M17" s="4">
-        <v>20.0</v>
-      </c>
-      <c r="N17" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="O17" s="4">
-        <v>6.0</v>
-      </c>
-      <c r="P17" s="4">
         <v>55.0</v>
       </c>
     </row>
@@ -1223,37 +1093,28 @@
       <c r="E18" s="4">
         <v>3.0</v>
       </c>
-      <c r="F18" s="4">
-        <v>3.0</v>
+      <c r="F18" s="7">
+        <v>2.0</v>
       </c>
       <c r="G18" s="4">
         <v>4.0</v>
       </c>
       <c r="H18" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="I18" s="4">
-        <v>4.0</v>
+        <v>3.0</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J18" s="4">
-        <v>3.0</v>
+        <v>20.0</v>
       </c>
       <c r="K18" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>16</v>
+        <v>0.0</v>
+      </c>
+      <c r="L18" s="4">
+        <v>6.0</v>
       </c>
       <c r="M18" s="4">
-        <v>20.0</v>
-      </c>
-      <c r="N18" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="O18" s="4">
-        <v>6.0</v>
-      </c>
-      <c r="P18" s="4">
         <v>56.0</v>
       </c>
     </row>
@@ -1273,37 +1134,28 @@
       <c r="E19" s="4">
         <v>2.0</v>
       </c>
-      <c r="F19" s="4">
-        <v>2.0</v>
+      <c r="F19" s="7">
+        <v>1.0</v>
       </c>
       <c r="G19" s="4">
         <v>3.0</v>
       </c>
       <c r="H19" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="I19" s="4">
-        <v>3.0</v>
+        <v>3.0</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J19" s="4">
-        <v>3.0</v>
+        <v>20.0</v>
       </c>
       <c r="K19" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>16</v>
+        <v>0.0</v>
+      </c>
+      <c r="L19" s="4">
+        <v>6.0</v>
       </c>
       <c r="M19" s="4">
-        <v>20.0</v>
-      </c>
-      <c r="N19" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="O19" s="4">
-        <v>6.0</v>
-      </c>
-      <c r="P19" s="4">
         <v>56.0</v>
       </c>
     </row>
@@ -1323,37 +1175,28 @@
       <c r="E20" s="4">
         <v>2.0</v>
       </c>
-      <c r="F20" s="4">
-        <v>2.0</v>
+      <c r="F20" s="7">
+        <v>1.0</v>
       </c>
       <c r="G20" s="4">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H20" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="I20" s="4">
-        <v>3.0</v>
+        <v>2.0</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J20" s="4">
-        <v>2.0</v>
+        <v>20.0</v>
       </c>
       <c r="K20" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="L20" s="4" t="s">
-        <v>16</v>
+        <v>0.0</v>
+      </c>
+      <c r="L20" s="4">
+        <v>6.0</v>
       </c>
       <c r="M20" s="4">
-        <v>20.0</v>
-      </c>
-      <c r="N20" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="O20" s="4">
-        <v>6.0</v>
-      </c>
-      <c r="P20" s="4">
         <v>54.0</v>
       </c>
     </row>
@@ -1373,37 +1216,28 @@
       <c r="E21" s="4">
         <v>3.0</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="7">
         <v>2.0</v>
       </c>
       <c r="G21" s="4">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H21" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="I21" s="4">
-        <v>2.0</v>
+        <v>4.0</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J21" s="4">
-        <v>4.0</v>
+        <v>21.0</v>
       </c>
       <c r="K21" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="L21" s="4" t="s">
+        <v>5.0</v>
+      </c>
+      <c r="L21" s="8" t="s">
         <v>16</v>
       </c>
       <c r="M21" s="4">
-        <v>21.0</v>
-      </c>
-      <c r="N21" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="O21" s="4">
-        <v>16.0</v>
-      </c>
-      <c r="P21" s="4">
         <v>64.0</v>
       </c>
     </row>
@@ -1423,37 +1257,28 @@
       <c r="E22" s="4">
         <v>1.0</v>
       </c>
-      <c r="F22" s="4">
-        <v>1.0</v>
+      <c r="F22" s="7">
+        <v>2.0</v>
       </c>
       <c r="G22" s="4">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H22" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="I22" s="4">
-        <v>3.0</v>
+        <v>3.0</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J22" s="4">
-        <v>3.0</v>
+        <v>21.0</v>
       </c>
       <c r="K22" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="L22" s="4" t="s">
+        <v>5.0</v>
+      </c>
+      <c r="L22" s="8" t="s">
         <v>16</v>
       </c>
       <c r="M22" s="4">
-        <v>21.0</v>
-      </c>
-      <c r="N22" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="O22" s="4">
-        <v>16.0</v>
-      </c>
-      <c r="P22" s="4">
         <v>63.0</v>
       </c>
     </row>
@@ -1473,37 +1298,28 @@
       <c r="E23" s="4">
         <v>2.0</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="7">
         <v>1.0</v>
       </c>
       <c r="G23" s="4">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H23" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="I23" s="4">
-        <v>3.0</v>
+        <v>2.0</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J23" s="4">
-        <v>2.0</v>
+        <v>21.0</v>
       </c>
       <c r="K23" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="L23" s="4" t="s">
+        <v>5.0</v>
+      </c>
+      <c r="L23" s="8" t="s">
         <v>16</v>
       </c>
       <c r="M23" s="4">
-        <v>21.0</v>
-      </c>
-      <c r="N23" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="O23" s="4">
-        <v>16.0</v>
-      </c>
-      <c r="P23" s="4">
         <v>62.0</v>
       </c>
     </row>
@@ -1523,8 +1339,8 @@
       <c r="E24" s="4">
         <v>3.0</v>
       </c>
-      <c r="F24" s="4">
-        <v>3.0</v>
+      <c r="F24" s="7">
+        <v>2.0</v>
       </c>
       <c r="G24" s="4">
         <v>3.0</v>
@@ -1532,28 +1348,19 @@
       <c r="H24" s="4">
         <v>2.0</v>
       </c>
-      <c r="I24" s="4">
-        <v>3.0</v>
+      <c r="I24" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J24" s="4">
-        <v>2.0</v>
+        <v>22.0</v>
       </c>
       <c r="K24" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="L24" s="4" t="s">
+        <v>6.0</v>
+      </c>
+      <c r="L24" s="8" t="s">
         <v>16</v>
       </c>
       <c r="M24" s="4">
-        <v>22.0</v>
-      </c>
-      <c r="N24" s="4">
-        <v>6.0</v>
-      </c>
-      <c r="O24" s="4">
-        <v>16.0</v>
-      </c>
-      <c r="P24" s="4">
         <v>61.0</v>
       </c>
     </row>
@@ -1573,37 +1380,28 @@
       <c r="E25" s="4">
         <v>1.0</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25" s="7">
         <v>2.0</v>
       </c>
       <c r="G25" s="4">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="H25" s="4">
         <v>2.0</v>
       </c>
-      <c r="I25" s="4">
-        <v>2.0</v>
+      <c r="I25" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J25" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="K25" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="L25" s="4" t="s">
+        <v>14.0</v>
+      </c>
+      <c r="K25" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="L25" s="8" t="s">
         <v>16</v>
       </c>
       <c r="M25" s="4">
-        <v>14.0</v>
-      </c>
-      <c r="N25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O25" s="4">
-        <v>16.0</v>
-      </c>
-      <c r="P25" s="4">
         <v>65.0</v>
       </c>
     </row>
@@ -1618,42 +1416,33 @@
         <v>45086.0</v>
       </c>
       <c r="D26" s="6">
-        <v>0.0</v>
+        <v>0.5</v>
       </c>
       <c r="E26" s="4">
         <v>2.0</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F26" s="7">
         <v>2.0</v>
       </c>
       <c r="G26" s="4">
         <v>2.0</v>
       </c>
       <c r="H26" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="I26" s="4">
-        <v>2.0</v>
+        <v>4.0</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J26" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="K26" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="L26" s="4" t="s">
+        <v>21.0</v>
+      </c>
+      <c r="K26" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="L26" s="8" t="s">
         <v>16</v>
       </c>
       <c r="M26" s="4">
-        <v>21.0</v>
-      </c>
-      <c r="N26" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O26" s="4">
-        <v>16.0</v>
-      </c>
-      <c r="P26" s="4">
         <v>65.0</v>
       </c>
     </row>
@@ -1667,43 +1456,34 @@
       <c r="C27" s="5">
         <v>45086.0</v>
       </c>
-      <c r="D27" s="6">
-        <v>0.011111111110949423</v>
+      <c r="D27" s="9">
+        <v>0.51875</v>
       </c>
       <c r="E27" s="4">
         <v>3.0</v>
       </c>
-      <c r="F27" s="4">
-        <v>3.0</v>
+      <c r="F27" s="7">
+        <v>2.0</v>
       </c>
       <c r="G27" s="4">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H27" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="I27" s="4">
-        <v>2.0</v>
+        <v>3.0</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J27" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="K27" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="L27" s="4" t="s">
+        <v>21.0</v>
+      </c>
+      <c r="K27" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="L27" s="8" t="s">
         <v>16</v>
       </c>
       <c r="M27" s="4">
-        <v>21.0</v>
-      </c>
-      <c r="N27" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O27" s="4">
-        <v>16.0</v>
-      </c>
-      <c r="P27" s="4">
         <v>65.0</v>
       </c>
     </row>
@@ -1717,13 +1497,13 @@
       <c r="C28" s="5">
         <v>45086.0</v>
       </c>
-      <c r="D28" s="6">
-        <v>0.011805555557657499</v>
+      <c r="D28" s="9">
+        <v>0.5263888888888889</v>
       </c>
       <c r="E28" s="4">
         <v>2.0</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F28" s="7">
         <v>3.0</v>
       </c>
       <c r="G28" s="4">
@@ -1732,28 +1512,19 @@
       <c r="H28" s="4">
         <v>3.0</v>
       </c>
-      <c r="I28" s="4">
-        <v>3.0</v>
+      <c r="I28" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J28" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="K28" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="L28" s="4" t="s">
+        <v>21.0</v>
+      </c>
+      <c r="K28" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="L28" s="8" t="s">
         <v>16</v>
       </c>
       <c r="M28" s="4">
-        <v>21.0</v>
-      </c>
-      <c r="N28" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O28" s="4">
-        <v>16.0</v>
-      </c>
-      <c r="P28" s="4">
         <v>65.0</v>
       </c>
     </row>
@@ -1773,8 +1544,8 @@
       <c r="E29" s="4">
         <v>3.0</v>
       </c>
-      <c r="F29" s="4">
-        <v>3.0</v>
+      <c r="F29" s="7">
+        <v>4.0</v>
       </c>
       <c r="G29" s="4">
         <v>3.0</v>
@@ -1782,84 +1553,66 @@
       <c r="H29" s="4">
         <v>4.0</v>
       </c>
-      <c r="I29" s="4">
-        <v>3.0</v>
+      <c r="I29" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J29" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="K29" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="L29" s="4" t="s">
+        <v>21.0</v>
+      </c>
+      <c r="K29" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="L29" s="8" t="s">
         <v>16</v>
       </c>
       <c r="M29" s="4">
-        <v>21.0</v>
-      </c>
-      <c r="N29" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O29" s="4">
-        <v>16.0</v>
-      </c>
-      <c r="P29" s="4">
         <v>65.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3">
-        <v>45086.845750520835</v>
+        <v>45086.57655092593</v>
       </c>
       <c r="B30" s="4">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C30" s="5">
         <v>45086.0</v>
       </c>
       <c r="D30" s="6">
-        <v>0.8402777777810115</v>
+        <v>0.5777777777777777</v>
       </c>
       <c r="E30" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="F30" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F30" s="7">
         <v>4.0</v>
       </c>
       <c r="G30" s="4">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="H30" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="I30" s="4">
-        <v>4.0</v>
+        <v>4.0</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J30" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="K30" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="L30" s="4" t="s">
+        <v>21.0</v>
+      </c>
+      <c r="K30" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="L30" s="8" t="s">
         <v>16</v>
       </c>
       <c r="M30" s="4">
-        <v>27.0</v>
-      </c>
-      <c r="N30" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="O30" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="P30" s="4">
-        <v>46.0</v>
+        <v>65.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3">
-        <v>45086.85284465278</v>
+        <v>45086.845750520835</v>
       </c>
       <c r="B31" s="4">
         <v>1.0</v>
@@ -1868,42 +1621,74 @@
         <v>45086.0</v>
       </c>
       <c r="D31" s="6">
+        <v>0.8402777777810115</v>
+      </c>
+      <c r="E31" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F31" s="7">
+        <v>3.0</v>
+      </c>
+      <c r="G31" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="H31" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J31" s="4">
+        <v>27.0</v>
+      </c>
+      <c r="K31" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="L31" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="M31" s="4">
+        <v>46.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="3">
+        <v>45086.85284465278</v>
+      </c>
+      <c r="B32" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C32" s="5">
+        <v>45086.0</v>
+      </c>
+      <c r="D32" s="6">
         <v>0.8486111111124046</v>
       </c>
-      <c r="E31" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="F31" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="G31" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="H31" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="I31" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="J31" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="K31" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="L31" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M31" s="4">
+      <c r="E32" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F32" s="7">
+        <v>3.0</v>
+      </c>
+      <c r="G32" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="H32" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J32" s="4">
         <v>26.0</v>
       </c>
-      <c r="N31" s="4">
+      <c r="K32" s="4">
         <v>0.0</v>
       </c>
-      <c r="O31" s="4">
+      <c r="L32" s="4">
         <v>5.0</v>
       </c>
-      <c r="P31" s="4">
+      <c r="M32" s="4">
         <v>46.0</v>
       </c>
     </row>
@@ -1939,22 +1724,22 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2">

</xml_diff>